<commit_message>
Prueba de recurso Generico
</commit_message>
<xml_diff>
--- a/Library_benchmark/Resource/BookEPPLUS.xlsx
+++ b/Library_benchmark/Resource/BookEPPLUS.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -23,7 +23,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,6 +33,13 @@
     </font>
     <font>
       <sz val="72"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -65,11 +72,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,15 +415,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C1:O6"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:O6"/>
+      <selection activeCell="A8" sqref="A8:Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="3:15">
+    <row r="1" spans="1:26">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,7 +440,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="3:15">
+    <row r="2" spans="1:26">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -447,7 +455,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="3:15">
+    <row r="3" spans="1:26">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -462,7 +470,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="3:15">
+    <row r="4" spans="1:26">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -477,7 +485,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="3:15">
+    <row r="5" spans="1:26">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -492,7 +500,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="3:15">
+    <row r="6" spans="1:26">
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -507,6 +515,34 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
+    <row r="8" spans="1:26">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:O6"/>

</xml_diff>